<commit_message>
Cambios en el tamaño de etiqueta
se ajusto el tamaño de la etiqueta para que quede a la medida del la impresora
</commit_message>
<xml_diff>
--- a/Etiquetas/Files/Etiquetas.xlsx
+++ b/Etiquetas/Files/Etiquetas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Ubicaciones</t>
   </si>
@@ -35,43 +35,7 @@
     <t>xe001b</t>
   </si>
   <si>
-    <t>xe001c</t>
-  </si>
-  <si>
-    <t>xe001d</t>
-  </si>
-  <si>
-    <t>xe001e</t>
-  </si>
-  <si>
     <t>Loc</t>
-  </si>
-  <si>
-    <t>xe001f</t>
-  </si>
-  <si>
-    <t>xe001g</t>
-  </si>
-  <si>
-    <t>xe001h</t>
-  </si>
-  <si>
-    <t>xe001i</t>
-  </si>
-  <si>
-    <t>xe001j</t>
-  </si>
-  <si>
-    <t>xe001k</t>
-  </si>
-  <si>
-    <t>xe001l</t>
-  </si>
-  <si>
-    <t>xe001m</t>
-  </si>
-  <si>
-    <t>xe001n</t>
   </si>
 </sst>
 </file>
@@ -389,10 +353,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,7 +369,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -422,116 +386,8 @@
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B15" si="0">"_"&amp;A3</f>
+        <f>"_"&amp;A3</f>
         <v>_xe001b</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v>_xe001c</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="str">
-        <f t="shared" si="0"/>
-        <v>_xe001d</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="str">
-        <f t="shared" si="0"/>
-        <v>_xe001e</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="str">
-        <f t="shared" si="0"/>
-        <v>_xe001f</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>_xe001g</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="str">
-        <f t="shared" si="0"/>
-        <v>_xe001h</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="str">
-        <f t="shared" si="0"/>
-        <v>_xe001i</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="str">
-        <f t="shared" si="0"/>
-        <v>_xe001j</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="str">
-        <f t="shared" si="0"/>
-        <v>_xe001k</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="str">
-        <f t="shared" si="0"/>
-        <v>_xe001l</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="str">
-        <f t="shared" si="0"/>
-        <v>_xe001m</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="str">
-        <f t="shared" si="0"/>
-        <v>_xe001n</v>
       </c>
     </row>
   </sheetData>

</xml_diff>